<commit_message>
spreadsheet as valuesets, added testcases, refactor
</commit_message>
<xml_diff>
--- a/layers/cmd/testdata/valueset_sample.xlsx
+++ b/layers/cmd/testdata/valueset_sample.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+  <si>
+    <t>options.lookupOrder</t>
+  </si>
   <si>
     <t>CODE</t>
   </si>
@@ -22,6 +25,15 @@
     <t>DESCRIPTIVE_TEXT</t>
   </si>
   <si>
+    <t>options.separator</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>A2:CODE</t>
   </si>
   <si>
@@ -34,10 +46,10 @@
     <t>B3:DESCRIPTIVE_TEXT</t>
   </si>
   <si>
-    <t>A4:CODE</t>
-  </si>
-  <si>
-    <t>B4:DESCRIPTIVE_TEXT</t>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>X; Y; Z</t>
   </si>
 </sst>
 </file>
@@ -45,19 +57,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -93,31 +99,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,7 +436,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A3" ySplit="2" xSplit="0"/>
@@ -429,117 +444,171 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="29.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="29.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="25.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="30.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="27.649999999999995" customFormat="1" s="1">
-      <c r="A1" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.45" customFormat="1" s="1">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="27.649999999999995" customFormat="1" s="3">
       <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.45" customFormat="1" s="3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25" customFormat="1" s="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="C4" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="3">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A7" s="4"/>
-      <c r="B7" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A8" s="4"/>
-      <c r="B8" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A9" s="4"/>
-      <c r="B9" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A10" s="4"/>
-      <c r="B10" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A11" s="4"/>
-      <c r="B11" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A12" s="4"/>
-      <c r="B12" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A13" s="4"/>
-      <c r="B13" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A14" s="4"/>
-      <c r="B14" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A15" s="4"/>
-      <c r="B15" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A16" s="4"/>
-      <c r="B16" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A17" s="4"/>
-      <c r="B17" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="3">
       <c r="A18" s="4"/>
-      <c r="B18" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25" customFormat="1" s="3">
       <c r="A19" s="4"/>
-      <c r="B19" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25" customFormat="1" s="3">
       <c r="A20" s="4"/>
-      <c r="B20" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25" customFormat="1" s="3">
       <c r="A21" s="4"/>
-      <c r="B21" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25" customFormat="1" s="3">
       <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25" customFormat="1" s="3">
       <c r="A23" s="4"/>
-      <c r="B23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25" customFormat="1" s="3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25" customFormat="1" s="3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
spreadsheet as valuesets, added testcases, valueset lookup support, refactor
</commit_message>
<xml_diff>
--- a/layers/cmd/testdata/valueset_sample.xlsx
+++ b/layers/cmd/testdata/valueset_sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>options.lookupOrder</t>
   </si>
@@ -99,12 +99,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
@@ -450,11 +453,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="29.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="25.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="19.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="25.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="26.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="29.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="25.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="14" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="25.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="26.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -467,8 +470,10 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -489,194 +494,194 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="27.649999999999995" customFormat="1" s="4">
-      <c r="A3" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="27.649999999999995" customFormat="1" s="5">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.45" customFormat="1" s="4">
-      <c r="A4" s="5" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.45" customFormat="1" s="5">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A5" s="5" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A6" s="5" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="4">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25" customFormat="1" s="4">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25" customFormat="1" s="4">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25" customFormat="1" s="4">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25" customFormat="1" s="4">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25" customFormat="1" s="4">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25" customFormat="1" s="4">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="11"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25" customFormat="1" s="4">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="11"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A17" s="6"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="5">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25" customFormat="1" s="5">
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25" customFormat="1" s="5">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25" customFormat="1" s="5">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25" customFormat="1" s="5">
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25" customFormat="1" s="5">
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25" customFormat="1" s="5">
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="12"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25" customFormat="1" s="5">
+      <c r="A25" s="6"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>